<commit_message>
Updated current consumption estimation
</commit_message>
<xml_diff>
--- a/doc/FridgeAlarm Current Consumption.xlsx
+++ b/doc/FridgeAlarm Current Consumption.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -18,12 +18,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Andreas</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Andreas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Measured for 600 Hz with 10% duty cycle.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
-    <t>Barrery capacity</t>
-  </si>
-  <si>
     <t>mA</t>
   </si>
   <si>
@@ -106,6 +139,9 @@
   </si>
   <si>
     <t>Blink period</t>
+  </si>
+  <si>
+    <t>Battery capacity</t>
   </si>
 </sst>
 </file>
@@ -113,9 +149,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +177,21 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,7 +229,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
@@ -522,11 +573,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -536,241 +587,241 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1">
         <v>2000</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>2.4E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2.2000000000000002</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3">
         <f>(3600*24-B10*B12-B11/7*B13)</f>
-        <v>86173.571428571435</v>
+        <v>86172.142857142855</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2">
         <v>0.1</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3">
         <f>B14/B16*B15</f>
-        <v>1077.1696428571429</v>
+        <v>1077.1517857142858</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="3">
         <f>B14-B17</f>
-        <v>85096.40178571429</v>
+        <v>85094.991071428565</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1">
         <f>B10*B12/3600*B5*7</f>
         <v>0.96250000000000013</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1">
         <f>B13*B11/3600*B6</f>
-        <v>1.388888888888889E-2</v>
+        <v>1.9444444444444445E-2</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1">
         <f>B17*B5/3600*7</f>
-        <v>4.6078923611111113</v>
+        <v>4.6078159722222223</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
         <f>B18*B4/3600*7</f>
-        <v>3.971165416666667</v>
+        <v>3.9710995833333333</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
         <f>SUM(B21:B24)</f>
-        <v>9.5554466666666666</v>
+        <v>9.5608599999999999</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="3">
         <f>B1/B25*7</f>
-        <v>1465.1329747711079</v>
+        <v>1464.3034204036039</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2">
         <f>B27/365</f>
-        <v>4.0140629445783782</v>
+        <v>4.0117901928865862</v>
       </c>
     </row>
   </sheetData>
@@ -787,7 +838,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>